<commit_message>
Updating as on 4/15/2019
</commit_message>
<xml_diff>
--- a/finance.xlsx
+++ b/finance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AP00595945\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -411,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -440,10 +440,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -794,11 +790,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="28"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -811,24 +807,24 @@
         <v>2</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="24">
+      <c r="A3" s="22">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="22">
         <v>1908</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="23" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="7">
@@ -836,19 +832,19 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="24">
+      <c r="A4" s="22">
         <v>2</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="22">
         <v>1972</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="23" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="7">
@@ -856,19 +852,19 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="24">
+      <c r="A5" s="22">
         <v>3</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="22">
         <v>2000</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="23" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="7">
@@ -876,19 +872,19 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="24">
+      <c r="A6" s="22">
         <v>4</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="22">
         <v>4000</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="23" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="7">
@@ -896,19 +892,19 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="24">
+      <c r="A7" s="22">
         <v>5</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="22">
         <v>6000</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="23" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="7">
@@ -928,25 +924,25 @@
       <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="22"/>
+      <c r="E8" s="20"/>
       <c r="G8" s="7">
         <v>20000</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
+      <c r="A9" s="22">
         <v>7</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="22">
         <v>20000</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="23" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="7">
@@ -954,19 +950,19 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="24">
+      <c r="A10" s="22">
         <v>8</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="22">
         <v>24000</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="23" t="s">
         <v>21</v>
       </c>
       <c r="G10">
@@ -987,30 +983,30 @@
       <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="22"/>
+      <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
+      <c r="A12" s="22">
         <v>10</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="22">
         <v>50000</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="23" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="27"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="2">
         <f>SUM(C3:C12)</f>
         <v>166880</v>
@@ -1082,11 +1078,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1198,10 +1194,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="33"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="1">
         <f>SUM(C3:C9)</f>
         <v>59880</v>
@@ -1234,13 +1230,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1409,10 +1405,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="35"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="10">
         <f>SUM(C3:C11)</f>
         <v>59298.5</v>
@@ -1460,13 +1456,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1623,10 +1619,10 @@
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="35"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="10">
         <f>SUM(C3:C11)</f>
         <v>45575.5</v>
@@ -1645,13 +1641,13 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
       <c r="I19" s="5" t="s">
         <v>47</v>
       </c>
@@ -1848,13 +1844,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2011,15 +2007,15 @@
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="35"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="10">
         <f>SUM(C3:C11)</f>
         <v>36845</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="19">
         <f>(D16)-SUM(D3:D11)-D28</f>
         <v>3312</v>
       </c>
@@ -2031,16 +2027,16 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -2058,9 +2054,9 @@
       <c r="E20" s="8">
         <v>43528</v>
       </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -2078,9 +2074,9 @@
       <c r="E21" s="8">
         <v>43529</v>
       </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
@@ -2098,9 +2094,9 @@
       <c r="E22" s="8">
         <v>43536</v>
       </c>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
@@ -2185,7 +2181,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,28 +2196,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="24" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2294,17 +2290,21 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="14">
         <v>5</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="14">
         <v>4237</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="18"/>
+      <c r="D7" s="16">
+        <v>4237</v>
+      </c>
+      <c r="E7" s="15">
+        <v>43570</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
@@ -2356,10 +2356,10 @@
         <v>800</v>
       </c>
       <c r="D11" s="13">
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="E11" s="8">
-        <v>43564</v>
+        <v>43570</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2373,24 +2373,24 @@
         <v>1500</v>
       </c>
       <c r="D12" s="13">
-        <v>501</v>
+        <v>707</v>
       </c>
       <c r="E12" s="8">
-        <v>43563</v>
+        <v>43570</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="35"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="10">
         <f>SUM(C3:C12)</f>
         <v>43811.57</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="19">
         <f>D17-SUM(D3:D12)-D29</f>
-        <v>5078.43</v>
+        <v>590.43000000000029</v>
       </c>
       <c r="E13" s="9"/>
     </row>
@@ -2400,16 +2400,16 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -2427,9 +2427,9 @@
       <c r="E21" s="8">
         <v>43553</v>
       </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
@@ -2447,9 +2447,9 @@
       <c r="E22" s="8">
         <v>43554</v>
       </c>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -2467,9 +2467,9 @@
       <c r="E23" s="8">
         <v>43554</v>
       </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="12">

</xml_diff>

<commit_message>
Updating as of 4/15/2019
</commit_message>
<xml_diff>
--- a/finance.xlsx
+++ b/finance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Debits" sheetId="1" r:id="rId1"/>
@@ -2181,7 +2181,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2356,7 +2356,7 @@
         <v>800</v>
       </c>
       <c r="D11" s="13">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="E11" s="8">
         <v>43570</v>
@@ -2373,7 +2373,7 @@
         <v>1500</v>
       </c>
       <c r="D12" s="13">
-        <v>707</v>
+        <v>767</v>
       </c>
       <c r="E12" s="8">
         <v>43570</v>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="D13" s="19">
         <f>D17-SUM(D3:D12)-D29</f>
-        <v>590.43000000000029</v>
+        <v>-1670.0599999999977</v>
       </c>
       <c r="E13" s="9"/>
     </row>
@@ -2530,13 +2530,13 @@
         <v>69</v>
       </c>
       <c r="C27" s="5">
-        <v>2000</v>
+        <v>4180.49</v>
       </c>
       <c r="D27" s="5">
-        <v>2000</v>
+        <v>4180.49</v>
       </c>
       <c r="E27" s="8">
-        <v>43564</v>
+        <v>43569</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D29">
         <f>SUM(D21:D28)</f>
-        <v>57878</v>
+        <v>60058.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating as of 4/18/2019 10:36AM
</commit_message>
<xml_diff>
--- a/finance.xlsx
+++ b/finance.xlsx
@@ -2181,7 +2181,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2356,10 +2356,10 @@
         <v>800</v>
       </c>
       <c r="D11" s="13">
-        <v>220</v>
+        <v>315</v>
       </c>
       <c r="E11" s="8">
-        <v>43570</v>
+        <v>43573</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2373,10 +2373,10 @@
         <v>1500</v>
       </c>
       <c r="D12" s="13">
-        <v>767</v>
+        <v>953</v>
       </c>
       <c r="E12" s="8">
-        <v>43570</v>
+        <v>43573</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2390,7 +2390,7 @@
       </c>
       <c r="D13" s="19">
         <f>D17-SUM(D3:D12)-D29</f>
-        <v>-1670.0599999999977</v>
+        <v>-1996.0599999999977</v>
       </c>
       <c r="E13" s="9"/>
     </row>
@@ -2496,13 +2496,13 @@
         <v>60</v>
       </c>
       <c r="C25" s="12">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="D25" s="12">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="E25" s="8">
-        <v>43556</v>
+        <v>43570</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D29">
         <f>SUM(D21:D28)</f>
-        <v>60058.49</v>
+        <v>60103.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating as of 10:12 AM
</commit_message>
<xml_diff>
--- a/finance.xlsx
+++ b/finance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Debits" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="March '19" sheetId="5" r:id="rId5"/>
     <sheet name="Apr '19" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="71">
   <si>
     <t>Sl No</t>
   </si>
@@ -239,12 +239,15 @@
   </si>
   <si>
     <t>Suraj</t>
+  </si>
+  <si>
+    <t>Samad Housewarming</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2181,7 +2184,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2356,10 +2359,10 @@
         <v>800</v>
       </c>
       <c r="D11" s="13">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="E11" s="8">
-        <v>43573</v>
+        <v>43574</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2373,10 +2376,10 @@
         <v>1500</v>
       </c>
       <c r="D12" s="13">
-        <v>953</v>
+        <v>993</v>
       </c>
       <c r="E12" s="8">
-        <v>43573</v>
+        <v>43574</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2390,7 +2393,7 @@
       </c>
       <c r="D13" s="19">
         <f>D17-SUM(D3:D12)-D29</f>
-        <v>-1996.0599999999977</v>
+        <v>-12056.05999999999</v>
       </c>
       <c r="E13" s="9"/>
     </row>
@@ -2540,16 +2543,26 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="8"/>
+      <c r="A28" s="12">
+        <v>7</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="12">
+        <v>10000</v>
+      </c>
+      <c r="D28" s="12">
+        <v>10000</v>
+      </c>
+      <c r="E28" s="8">
+        <v>43574</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D29">
         <f>SUM(D21:D28)</f>
-        <v>60103.49</v>
+        <v>70103.489999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating as of 4/21/2019 9:24PM
</commit_message>
<xml_diff>
--- a/finance.xlsx
+++ b/finance.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AP00595945\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="5"/>
   </bookViews>
@@ -19,9 +14,9 @@
     <sheet name="March '19" sheetId="5" r:id="rId5"/>
     <sheet name="Apr '19" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="72">
   <si>
     <t>Sl No</t>
   </si>
@@ -242,13 +237,16 @@
   </si>
   <si>
     <t>Samad Housewarming</t>
+  </si>
+  <si>
+    <t>Dmart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,7 +555,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -592,7 +590,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -769,21 +767,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -792,14 +790,14 @@
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="26" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="28"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,7 +812,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="22">
         <v>1</v>
       </c>
@@ -834,7 +832,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="22">
         <v>2</v>
       </c>
@@ -854,7 +852,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="22">
         <v>3</v>
       </c>
@@ -874,7 +872,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="22">
         <v>4</v>
       </c>
@@ -894,7 +892,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="22">
         <v>5</v>
       </c>
@@ -914,7 +912,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -932,7 +930,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="22">
         <v>7</v>
       </c>
@@ -952,7 +950,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="22">
         <v>8</v>
       </c>
@@ -973,7 +971,7 @@
         <v>59880</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -988,7 +986,7 @@
       </c>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="22">
         <v>10</v>
       </c>
@@ -1005,7 +1003,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="25" t="s">
         <v>13</v>
       </c>
@@ -1015,12 +1013,12 @@
         <v>166880</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="G14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="F15" t="s">
         <v>64</v>
       </c>
@@ -1028,7 +1026,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="F16" t="s">
         <v>65</v>
       </c>
@@ -1036,7 +1034,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:7">
       <c r="F17" t="s">
         <v>66</v>
       </c>
@@ -1044,7 +1042,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:7">
       <c r="F18" t="s">
         <v>67</v>
       </c>
@@ -1066,28 +1064,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1112,7 +1110,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -1126,7 +1124,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -1140,7 +1138,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -1154,7 +1152,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -1168,7 +1166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -1182,7 +1180,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1196,7 +1194,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="30" t="s">
         <v>13</v>
       </c>
@@ -1217,14 +1215,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1232,7 +1230,7 @@
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="34" t="s">
         <v>22</v>
       </c>
@@ -1241,7 +1239,7 @@
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1258,7 +1256,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="14">
         <v>1</v>
       </c>
@@ -1275,7 +1273,7 @@
         <v>43471</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="14">
         <v>2</v>
       </c>
@@ -1292,7 +1290,7 @@
         <v>43470</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="14">
         <v>3</v>
       </c>
@@ -1309,7 +1307,7 @@
         <v>43468</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="14">
         <v>4</v>
       </c>
@@ -1326,7 +1324,7 @@
         <v>43480</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="14">
         <v>5</v>
       </c>
@@ -1343,7 +1341,7 @@
         <v>43470</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="14">
         <v>6</v>
       </c>
@@ -1360,7 +1358,7 @@
         <v>43471</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1375,7 +1373,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1390,7 +1388,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -1407,7 +1405,7 @@
         <v>43469</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="32" t="s">
         <v>34</v>
       </c>
@@ -1424,7 +1422,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="D15" s="11">
         <v>60056</v>
       </c>
@@ -1440,14 +1438,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1458,7 +1456,7 @@
     <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="34" t="s">
         <v>36</v>
       </c>
@@ -1467,7 +1465,7 @@
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1484,7 +1482,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="14">
         <v>1</v>
       </c>
@@ -1501,7 +1499,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="14">
         <v>2</v>
       </c>
@@ -1518,7 +1516,7 @@
         <v>43501</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="14">
         <v>3</v>
       </c>
@@ -1535,7 +1533,7 @@
         <v>43503</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="14">
         <v>4</v>
       </c>
@@ -1552,7 +1550,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="14">
         <v>5</v>
       </c>
@@ -1569,7 +1567,7 @@
         <v>43501</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -1582,7 +1580,7 @@
       <c r="D8" s="13"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1595,7 +1593,7 @@
       <c r="D9" s="13"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1608,7 +1606,7 @@
       <c r="D10" s="13"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1621,7 +1619,7 @@
       <c r="D11" s="13"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="32" t="s">
         <v>34</v>
       </c>
@@ -1638,12 +1636,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="D16" s="5">
         <v>60782</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="35" t="s">
         <v>39</v>
       </c>
@@ -1658,7 +1656,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="5">
         <v>1</v>
       </c>
@@ -1681,7 +1679,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="5">
         <v>2</v>
       </c>
@@ -1704,7 +1702,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="5">
         <v>3</v>
       </c>
@@ -1725,7 +1723,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="12">
         <v>4</v>
       </c>
@@ -1742,7 +1740,7 @@
         <v>43499</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="12">
         <v>5</v>
       </c>
@@ -1759,7 +1757,7 @@
         <v>43505</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="12">
         <v>6</v>
       </c>
@@ -1776,7 +1774,7 @@
         <v>43505</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="12">
         <v>7</v>
       </c>
@@ -1793,7 +1791,7 @@
         <v>43505</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="12">
         <v>8</v>
       </c>
@@ -1810,7 +1808,7 @@
         <v>43505</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="D28">
         <f>SUM(D20:D27)</f>
         <v>22019</v>
@@ -1828,14 +1826,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -1846,7 +1844,7 @@
     <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="30" t="s">
         <v>36</v>
       </c>
@@ -1855,7 +1853,7 @@
       <c r="D1" s="37"/>
       <c r="E1" s="31"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1872,7 +1870,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="14">
         <v>1</v>
       </c>
@@ -1889,7 +1887,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="14">
         <v>2</v>
       </c>
@@ -1906,7 +1904,7 @@
         <v>43529</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="14">
         <v>3</v>
       </c>
@@ -1923,7 +1921,7 @@
         <v>43529</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="14">
         <v>4</v>
       </c>
@@ -1940,7 +1938,7 @@
         <v>43539</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="14">
         <v>5</v>
       </c>
@@ -1957,7 +1955,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="17">
         <v>6</v>
       </c>
@@ -1968,7 +1966,7 @@
       <c r="D8" s="13"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="17">
         <v>7</v>
       </c>
@@ -1979,7 +1977,7 @@
       <c r="D9" s="13"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="17">
         <v>8</v>
       </c>
@@ -1994,7 +1992,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="17">
         <v>9</v>
       </c>
@@ -2009,7 +2007,7 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="32" t="s">
         <v>34</v>
       </c>
@@ -2024,12 +2022,12 @@
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="D16" s="5">
         <v>60787</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="35" t="s">
         <v>39</v>
       </c>
@@ -2041,7 +2039,7 @@
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="5">
         <v>1</v>
       </c>
@@ -2061,7 +2059,7 @@
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="5">
         <v>2</v>
       </c>
@@ -2081,7 +2079,7 @@
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="5">
         <v>3</v>
       </c>
@@ -2101,7 +2099,7 @@
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="12">
         <v>4</v>
       </c>
@@ -2118,7 +2116,7 @@
         <v>43540</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="12">
         <v>5</v>
       </c>
@@ -2135,7 +2133,7 @@
         <v>43551</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="12">
         <v>6</v>
       </c>
@@ -2144,7 +2142,7 @@
       <c r="D25" s="12"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="12">
         <v>7</v>
       </c>
@@ -2153,7 +2151,7 @@
       <c r="D26" s="12"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="12">
         <v>8</v>
       </c>
@@ -2162,7 +2160,7 @@
       <c r="D27" s="12"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="D28">
         <f>SUM(D20:D27)</f>
         <v>19868</v>
@@ -2180,14 +2178,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -2198,7 +2196,7 @@
     <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="30" t="s">
         <v>36</v>
       </c>
@@ -2207,7 +2205,7 @@
       <c r="D1" s="37"/>
       <c r="E1" s="31"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
@@ -2224,7 +2222,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="14">
         <v>1</v>
       </c>
@@ -2241,7 +2239,7 @@
         <v>43563</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="14">
         <v>2</v>
       </c>
@@ -2258,7 +2256,7 @@
         <v>43560</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="14">
         <v>3</v>
       </c>
@@ -2275,7 +2273,7 @@
         <v>43560</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="14">
         <v>4</v>
       </c>
@@ -2292,7 +2290,7 @@
         <v>43560</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="14">
         <v>5</v>
       </c>
@@ -2309,7 +2307,7 @@
         <v>43570</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="14">
         <v>6</v>
       </c>
@@ -2326,7 +2324,7 @@
         <v>43560</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="17">
         <v>7</v>
       </c>
@@ -2337,7 +2335,7 @@
       <c r="D9" s="13"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="17">
         <v>8</v>
       </c>
@@ -2348,7 +2346,7 @@
       <c r="D10" s="13"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="17">
         <v>9</v>
       </c>
@@ -2359,13 +2357,13 @@
         <v>800</v>
       </c>
       <c r="D11" s="13">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="E11" s="8">
-        <v>43574</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43576</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="17">
         <v>10</v>
       </c>
@@ -2376,13 +2374,13 @@
         <v>1500</v>
       </c>
       <c r="D12" s="13">
-        <v>993</v>
+        <v>1033</v>
       </c>
       <c r="E12" s="8">
-        <v>43574</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43576</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="32" t="s">
         <v>34</v>
       </c>
@@ -2392,17 +2390,17 @@
         <v>43811.57</v>
       </c>
       <c r="D13" s="19">
-        <f>D17-SUM(D3:D12)-D29</f>
-        <v>-12056.05999999999</v>
+        <f>D17-SUM(D3:D12)-D30</f>
+        <v>-12449.819999999985</v>
       </c>
       <c r="E13" s="9"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="D17" s="5">
         <v>100887</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="35" t="s">
         <v>39</v>
       </c>
@@ -2414,7 +2412,7 @@
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="5">
         <v>1</v>
       </c>
@@ -2434,7 +2432,7 @@
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="5">
         <v>2</v>
       </c>
@@ -2454,7 +2452,7 @@
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="5">
         <v>3</v>
       </c>
@@ -2474,7 +2472,7 @@
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="12">
         <v>4</v>
       </c>
@@ -2491,7 +2489,7 @@
         <v>43555</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="12">
         <v>6</v>
       </c>
@@ -2508,7 +2506,7 @@
         <v>43570</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="12">
         <v>5</v>
       </c>
@@ -2525,7 +2523,7 @@
         <v>43557</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="5">
         <v>6</v>
       </c>
@@ -2542,7 +2540,7 @@
         <v>43569</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="12">
         <v>7</v>
       </c>
@@ -2559,10 +2557,27 @@
         <v>43574</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D29">
-        <f>SUM(D21:D28)</f>
-        <v>70103.489999999991</v>
+    <row r="29" spans="1:11">
+      <c r="A29" s="12">
+        <v>8</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="12">
+        <v>338.76</v>
+      </c>
+      <c r="D29" s="12">
+        <v>338.76</v>
+      </c>
+      <c r="E29" s="8">
+        <v>43575</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="D30" s="5">
+        <f>SUM(D21:D29)</f>
+        <v>70442.249999999985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>